<commit_message>
modified:   "Hs ph\303\241t tri\341\273\203n s\341\272\243n ph\341\272\251m 5G Wifi/1. Router 4G Wifi/4G Wifi Huawei CPE vs No Huawei - technical compare (version 1).xlsb.xlsx"
</commit_message>
<xml_diff>
--- a/Hs phát triển sản phẩm 5G Wifi/1. Router 4G Wifi/4G Wifi Huawei CPE vs No Huawei - technical compare (version 1).xlsb.xlsx
+++ b/Hs phát triển sản phẩm 5G Wifi/1. Router 4G Wifi/4G Wifi Huawei CPE vs No Huawei - technical compare (version 1).xlsb.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\My\Desktop\Dung\thử việc mbf\Hs phát triển sản phẩm 5G Wifi\1. Router 4G Wifi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dzung\Desktop\mbf\thu_viec_mbf\Hs phát triển sản phẩm 5G Wifi\1. Router 4G Wifi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DC59E996-8442-4317-A53C-559475A1B377}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{037B33EF-1AE9-4DA6-8A6E-C9D465B18999}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="5G cpe " sheetId="4" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="B311-221(4G Wifi) vs NO Huawei" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="201">
   <si>
     <t>Product model</t>
   </si>
@@ -274,9 +273,6 @@
     <t>Với việc sở hữu cổng điện thoại chuẩn RJ, hỗ trợ tốt các tính năng CS/ VoLTE/ VoIP</t>
   </si>
   <si>
-    <t>Built-in antenna phù hợp hơn cho các Home Wifi vì độ phủ sóng đều hơn, gần như là hình cầu. Trong khi external antenna cho độ bao phủ mở rộng xa nhất từ phía nguồn phát.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Thiết kế nhỏ gọn hơn sản phẩm từ các đối thủ </t>
   </si>
   <si>
@@ -419,7 +415,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -428,7 +424,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -438,7 +434,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -450,7 +446,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -460,7 +456,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -570,10 +566,6 @@
 - Microphones, Speakers</t>
   </si>
   <si>
-    <t>-1 WAN GE port, 4LAN port
-- 1 x SIM card slot(for Nano-SIM card)</t>
-  </si>
-  <si>
     <t>Display</t>
   </si>
   <si>
@@ -708,17 +700,66 @@
     <t>WPS indicator (Led or LCD)
 WLAN indicator (Led or LCD)
 4 LAN indicator (Led or LCD)</t>
+  </si>
+  <si>
+    <t>- 1 WAN GE port,
+- 4 LAN ports
+- 1 x SIM card slot(for Nano-SIM card)
+- 1 power adapter port</t>
+  </si>
+  <si>
+    <t>Built-in antenna phù hợp hơn cho các Home Wifi vì độ phủ sóng đều hơn. Trong khi external antenna cho độ bao phủ mở rộng xa nhất từ phía nguồn phát.</t>
+  </si>
+  <si>
+    <t>SMS</t>
+  </si>
+  <si>
+    <t>IPv4/ipv6</t>
+  </si>
+  <si>
+    <t>CS/ VoLTE/ VoIP</t>
+  </si>
+  <si>
+    <t>1 power button
+1 reset button
+1 WPS button</t>
+  </si>
+  <si>
+    <t>1 led for 5G 
+1 led for 4G
+1 led for Wifi</t>
+  </si>
+  <si>
+    <t>IPv4 and IPv6/IPv4 dual stack</t>
+  </si>
+  <si>
+    <t>SMS service</t>
+  </si>
+  <si>
+    <t>firewall</t>
+  </si>
+  <si>
+    <t>PIN protection</t>
+  </si>
+  <si>
+    <t>MAC address filtering</t>
+  </si>
+  <si>
+    <t>VPN tunnel/VPN penetration</t>
+  </si>
+  <si>
+    <t>WebUI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -726,7 +767,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -765,7 +806,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -773,13 +814,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -813,6 +854,28 @@
       <color rgb="FF333333"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -953,7 +1016,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1054,6 +1117,29 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -1084,18 +1170,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1105,29 +1179,50 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1555,37 +1650,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFD3B9FB-EB72-43D1-8F21-9D6CE3B2B12D}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.7109375" customWidth="1"/>
-    <col min="4" max="4" width="50.28515625" customWidth="1"/>
-    <col min="5" max="5" width="47.140625" style="10" customWidth="1"/>
-    <col min="6" max="6" width="33.28515625" customWidth="1"/>
+    <col min="1" max="1" width="5.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.75" customWidth="1"/>
+    <col min="4" max="4" width="50.25" customWidth="1"/>
+    <col min="5" max="5" width="47.125" style="10" customWidth="1"/>
+    <col min="6" max="6" width="33.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="49.5">
       <c r="A1" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="C1" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="D1" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="E1" s="29" t="s">
         <v>127</v>
-      </c>
-      <c r="E1" s="29" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="16.5">
@@ -1593,36 +1688,36 @@
         <v>1</v>
       </c>
       <c r="B2" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" s="31" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="D2" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="D2" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="E2" s="31" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="198">
+      <c r="E2" s="56" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="181.5">
       <c r="A3" s="30">
         <v>2</v>
       </c>
       <c r="B3" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="C3" s="32" t="s">
         <v>132</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="D3" s="32" t="s">
         <v>133</v>
       </c>
-      <c r="D3" s="32" t="s">
-        <v>134</v>
-      </c>
-      <c r="E3" s="32" t="s">
-        <v>178</v>
-      </c>
-      <c r="F3" s="52" t="s">
-        <v>179</v>
+      <c r="E3" s="57" t="s">
+        <v>176</v>
+      </c>
+      <c r="F3" s="35" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.5">
@@ -1630,16 +1725,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="31" t="s">
+        <v>134</v>
+      </c>
+      <c r="C4" s="31" t="s">
         <v>135</v>
       </c>
-      <c r="C4" s="31" t="s">
-        <v>136</v>
-      </c>
       <c r="D4" s="31" t="s">
-        <v>136</v>
-      </c>
-      <c r="E4" s="31" t="s">
-        <v>136</v>
+        <v>135</v>
+      </c>
+      <c r="E4" s="56" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="99">
@@ -1647,53 +1742,53 @@
         <v>4</v>
       </c>
       <c r="B5" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="C5" s="32" t="s">
         <v>137</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="D5" s="32" t="s">
         <v>138</v>
       </c>
-      <c r="D5" s="32" t="s">
-        <v>139</v>
-      </c>
-      <c r="E5" s="32" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="49.5">
+      <c r="E5" s="57" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="33">
       <c r="A6" s="30">
         <v>5</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C6" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="D6" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" s="56" t="s">
         <v>140</v>
       </c>
-      <c r="D6" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="E6" s="31" t="s">
-        <v>141</v>
-      </c>
-      <c r="F6" s="51" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="66">
+      <c r="F6" s="34" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="49.5">
       <c r="A7" s="30">
         <v>6</v>
       </c>
       <c r="B7" s="31" t="s">
+        <v>141</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>180</v>
+      </c>
+      <c r="D7" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="C7" s="32" t="s">
-        <v>182</v>
-      </c>
-      <c r="D7" s="32" t="s">
-        <v>143</v>
-      </c>
-      <c r="E7" s="32" t="s">
-        <v>183</v>
+      <c r="E7" s="57" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="99">
@@ -1701,16 +1796,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="31" t="s">
+        <v>143</v>
+      </c>
+      <c r="C8" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="D8" s="32" t="s">
         <v>145</v>
       </c>
-      <c r="D8" s="32" t="s">
-        <v>146</v>
-      </c>
-      <c r="E8" s="32" t="s">
-        <v>147</v>
+      <c r="E8" s="57" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="33">
@@ -1718,16 +1813,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C9" s="32" t="s">
         <v>60</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>149</v>
-      </c>
-      <c r="E9" s="32" t="s">
-        <v>150</v>
+        <v>147</v>
+      </c>
+      <c r="E9" s="57" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16.5">
@@ -1735,15 +1830,15 @@
         <v>8</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D10" s="33">
         <v>20</v>
       </c>
-      <c r="E10" s="33">
+      <c r="E10" s="58">
         <v>50</v>
       </c>
     </row>
@@ -1752,16 +1847,16 @@
         <v>9</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="E11" s="32" t="s">
-        <v>153</v>
+        <v>100</v>
+      </c>
+      <c r="E11" s="57" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="33">
@@ -1769,16 +1864,16 @@
         <v>10</v>
       </c>
       <c r="B12" s="31" t="s">
+        <v>152</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="D12" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="E12" s="57" t="s">
         <v>154</v>
-      </c>
-      <c r="C12" s="32" t="s">
-        <v>155</v>
-      </c>
-      <c r="D12" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="E12" s="32" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16.5">
@@ -1786,16 +1881,16 @@
         <v>11</v>
       </c>
       <c r="B13" s="31" t="s">
+        <v>155</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="D13" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="E13" s="56" t="s">
         <v>157</v>
-      </c>
-      <c r="C13" s="31" t="s">
-        <v>158</v>
-      </c>
-      <c r="D13" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="E13" s="31" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="16.5">
@@ -1803,16 +1898,16 @@
         <v>12</v>
       </c>
       <c r="B14" s="31" t="s">
+        <v>158</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="D14" s="31" t="s">
         <v>160</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="E14" s="56" t="s">
         <v>161</v>
-      </c>
-      <c r="D14" s="31" t="s">
-        <v>162</v>
-      </c>
-      <c r="E14" s="31" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="16.5">
@@ -1820,16 +1915,16 @@
         <v>13</v>
       </c>
       <c r="B15" s="31" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C15" s="33">
         <v>600</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>165</v>
-      </c>
-      <c r="E15" s="31" t="s">
-        <v>166</v>
+        <v>163</v>
+      </c>
+      <c r="E15" s="56" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="16.5">
@@ -1837,52 +1932,165 @@
         <v>14</v>
       </c>
       <c r="B16" s="31" t="s">
+        <v>165</v>
+      </c>
+      <c r="C16" s="33" t="s">
+        <v>166</v>
+      </c>
+      <c r="D16" s="31" t="s">
         <v>167</v>
       </c>
-      <c r="C16" s="33" t="s">
-        <v>168</v>
-      </c>
-      <c r="D16" s="31" t="s">
-        <v>169</v>
-      </c>
-      <c r="E16" s="31"/>
-    </row>
-    <row r="17" spans="1:5" ht="45">
-      <c r="A17" s="54">
+      <c r="E16" s="56"/>
+    </row>
+    <row r="17" spans="1:5" ht="49.5">
+      <c r="A17" s="59">
         <v>15</v>
       </c>
-      <c r="B17" s="51" t="s">
-        <v>180</v>
-      </c>
-      <c r="E17" s="58" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="45">
-      <c r="A18" s="54">
+      <c r="B17" s="60" t="s">
+        <v>178</v>
+      </c>
+      <c r="C17" s="62" t="s">
+        <v>192</v>
+      </c>
+      <c r="D17" s="36"/>
+      <c r="E17" s="61" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="49.5">
+      <c r="A18" s="59">
         <v>16</v>
       </c>
-      <c r="B18" s="51" t="s">
-        <v>185</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>188</v>
+      <c r="B18" s="60" t="s">
+        <v>183</v>
+      </c>
+      <c r="C18" s="62" t="s">
+        <v>193</v>
+      </c>
+      <c r="D18" s="36"/>
+      <c r="E18" s="61" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16.5">
-      <c r="A19" s="59">
+      <c r="A19" s="67">
         <v>17</v>
       </c>
-      <c r="B19" s="51" t="s">
-        <v>43</v>
+      <c r="B19" s="64" t="s">
+        <v>184</v>
+      </c>
+      <c r="C19" s="70" t="s">
+        <v>195</v>
+      </c>
+      <c r="D19" s="36"/>
+      <c r="E19" s="61" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="16.5">
-      <c r="B20" s="57" t="s">
-        <v>186</v>
+      <c r="A20" s="68"/>
+      <c r="B20" s="65"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="61" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="16.5">
+      <c r="A21" s="68"/>
+      <c r="B21" s="65"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="61" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="16.5">
+      <c r="A22" s="68"/>
+      <c r="B22" s="65"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="63" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="16.5">
+      <c r="A23" s="68"/>
+      <c r="B23" s="65"/>
+      <c r="C23" s="71" t="s">
+        <v>194</v>
+      </c>
+      <c r="D23" s="36"/>
+      <c r="E23" s="61" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="16.5">
+      <c r="A24" s="68"/>
+      <c r="B24" s="65"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="63" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="16.5">
+      <c r="A25" s="68"/>
+      <c r="B25" s="65"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="61" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="16.5">
+      <c r="A26" s="69"/>
+      <c r="B26" s="66"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="61" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15">
+      <c r="C27" s="70" t="s">
+        <v>196</v>
+      </c>
+      <c r="E27" s="70" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15">
+      <c r="C28" s="70" t="s">
+        <v>197</v>
+      </c>
+      <c r="E28" s="70" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15">
+      <c r="C29" s="70" t="s">
+        <v>198</v>
+      </c>
+      <c r="E29" s="70" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15">
+      <c r="C30" s="70" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15">
+      <c r="C31" s="70" t="s">
+        <v>200</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B19:B26"/>
+    <mergeCell ref="A19:A26"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="D1" r:id="rId1" display="https://www.htc.com/vn/5g/htc-5g-hub/)" xr:uid="{EC2AE463-2BA2-4A7E-AF7A-05AD3688B96E}"/>
   </hyperlinks>
@@ -1895,17 +2103,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B86DDA3-AC0A-4D94-B436-44C073F25763}">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.7109375" customWidth="1"/>
-    <col min="4" max="4" width="51.85546875" customWidth="1"/>
-    <col min="5" max="5" width="53.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.75" customWidth="1"/>
+    <col min="4" max="4" width="51.875" customWidth="1"/>
+    <col min="5" max="5" width="53.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1920,7 +2128,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>66</v>
@@ -1934,230 +2142,230 @@
       <c r="C3" s="7"/>
       <c r="D3" s="18"/>
     </row>
-    <row r="4" spans="1:5">
-      <c r="B4" s="44" t="s">
+    <row r="4" spans="1:5" ht="15">
+      <c r="B4" s="39" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E4" s="9"/>
     </row>
-    <row r="5" spans="1:5" ht="30">
-      <c r="B5" s="44"/>
+    <row r="5" spans="1:5" ht="15">
+      <c r="B5" s="39"/>
       <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="B6" s="44"/>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15">
+      <c r="B6" s="39"/>
       <c r="C6" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E6" s="9"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="40" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>51</v>
       </c>
       <c r="D7" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="E7" s="9"/>
+    </row>
+    <row r="8" spans="1:5" ht="15">
+      <c r="B8" s="41"/>
+      <c r="C8" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="E7" s="9"/>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="B8" s="46"/>
-      <c r="C8" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>107</v>
-      </c>
       <c r="E8" s="9"/>
     </row>
-    <row r="9" spans="1:5" ht="30">
-      <c r="B9" s="46"/>
+    <row r="9" spans="1:5" ht="28.5">
+      <c r="B9" s="41"/>
       <c r="C9" s="4" t="s">
         <v>55</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="B10" s="46"/>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15">
+      <c r="B10" s="41"/>
       <c r="C10" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="30">
-      <c r="B11" s="46"/>
+      <c r="B11" s="41"/>
       <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="30">
-      <c r="B12" s="46"/>
+      <c r="B12" s="41"/>
       <c r="C12" s="4" t="s">
         <v>62</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E12" s="9"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="B13" s="46"/>
+      <c r="B13" s="41"/>
       <c r="C13" s="14" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E13" s="9"/>
     </row>
-    <row r="14" spans="1:5">
-      <c r="B14" s="46"/>
+    <row r="14" spans="1:5" ht="15">
+      <c r="B14" s="41"/>
       <c r="C14" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E14" s="9"/>
     </row>
-    <row r="15" spans="1:5">
-      <c r="B15" s="46"/>
+    <row r="15" spans="1:5" ht="15">
+      <c r="B15" s="41"/>
       <c r="C15" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E15" s="9"/>
     </row>
-    <row r="16" spans="1:5">
-      <c r="B16" s="46"/>
+    <row r="16" spans="1:5" ht="15">
+      <c r="B16" s="41"/>
       <c r="C16" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E16" s="9"/>
     </row>
-    <row r="17" spans="2:5">
-      <c r="B17" s="46"/>
+    <row r="17" spans="2:5" ht="15">
+      <c r="B17" s="41"/>
       <c r="C17" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E17" s="9"/>
     </row>
-    <row r="18" spans="2:5">
-      <c r="B18" s="46"/>
+    <row r="18" spans="2:5" ht="15">
+      <c r="B18" s="41"/>
       <c r="C18" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E18" s="9"/>
     </row>
-    <row r="19" spans="2:5">
-      <c r="B19" s="46"/>
+    <row r="19" spans="2:5" ht="15">
+      <c r="B19" s="41"/>
       <c r="C19" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E19" s="9"/>
     </row>
-    <row r="20" spans="2:5">
-      <c r="B20" s="46"/>
+    <row r="20" spans="2:5" ht="15">
+      <c r="B20" s="41"/>
       <c r="C20" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D20" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="21" spans="2:5">
-      <c r="B21" s="46"/>
+      <c r="B21" s="41"/>
       <c r="C21" s="14" t="s">
         <v>16</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="9"/>
     </row>
-    <row r="22" spans="2:5">
-      <c r="B22" s="46"/>
+    <row r="22" spans="2:5" ht="15">
+      <c r="B22" s="41"/>
       <c r="C22" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E22" s="9"/>
     </row>
-    <row r="23" spans="2:5">
-      <c r="B23" s="46"/>
+    <row r="23" spans="2:5" ht="15">
+      <c r="B23" s="41"/>
       <c r="C23" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E23" s="9"/>
     </row>
-    <row r="24" spans="2:5">
-      <c r="B24" s="46"/>
+    <row r="24" spans="2:5" ht="15">
+      <c r="B24" s="41"/>
       <c r="C24" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="25" spans="2:5">
-      <c r="B25" s="46"/>
+      <c r="B25" s="41"/>
       <c r="C25" s="14" t="s">
         <v>20</v>
       </c>
@@ -2166,134 +2374,134 @@
       </c>
       <c r="E25" s="9"/>
     </row>
-    <row r="26" spans="2:5">
-      <c r="B26" s="46"/>
+    <row r="26" spans="2:5" ht="15">
+      <c r="B26" s="41"/>
       <c r="C26" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="19"/>
       <c r="E26" s="9"/>
     </row>
-    <row r="27" spans="2:5">
-      <c r="B27" s="47"/>
+    <row r="27" spans="2:5" ht="15">
+      <c r="B27" s="42"/>
       <c r="C27" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D27" s="19"/>
       <c r="E27" s="9"/>
     </row>
-    <row r="28" spans="2:5">
-      <c r="B28" s="41" t="s">
+    <row r="28" spans="2:5" ht="15">
+      <c r="B28" s="50" t="s">
         <v>23</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E28" s="9"/>
     </row>
-    <row r="29" spans="2:5">
-      <c r="B29" s="42"/>
+    <row r="29" spans="2:5" ht="15">
+      <c r="B29" s="51"/>
       <c r="C29" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E29" s="9"/>
     </row>
-    <row r="30" spans="2:5">
-      <c r="B30" s="42"/>
+    <row r="30" spans="2:5" ht="15">
+      <c r="B30" s="51"/>
       <c r="C30" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D30" s="19"/>
       <c r="E30" s="9"/>
     </row>
-    <row r="31" spans="2:5">
-      <c r="B31" s="42"/>
+    <row r="31" spans="2:5" ht="15">
+      <c r="B31" s="51"/>
       <c r="C31" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D31" s="19"/>
       <c r="E31" s="9"/>
     </row>
-    <row r="32" spans="2:5">
-      <c r="B32" s="42"/>
+    <row r="32" spans="2:5" ht="15">
+      <c r="B32" s="51"/>
       <c r="C32" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D32" s="19"/>
       <c r="E32" s="9"/>
     </row>
-    <row r="33" spans="2:5">
-      <c r="B33" s="42"/>
+    <row r="33" spans="2:5" ht="15">
+      <c r="B33" s="51"/>
       <c r="C33" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D33" s="19"/>
       <c r="E33" s="9"/>
     </row>
-    <row r="34" spans="2:5">
-      <c r="B34" s="42"/>
+    <row r="34" spans="2:5" ht="15">
+      <c r="B34" s="51"/>
       <c r="C34" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D34" s="19"/>
       <c r="E34" s="9"/>
     </row>
-    <row r="35" spans="2:5">
-      <c r="B35" s="42"/>
+    <row r="35" spans="2:5" ht="15">
+      <c r="B35" s="51"/>
       <c r="C35" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D35" s="19"/>
       <c r="E35" s="9"/>
     </row>
-    <row r="36" spans="2:5">
-      <c r="B36" s="42"/>
+    <row r="36" spans="2:5" ht="15">
+      <c r="B36" s="51"/>
       <c r="C36" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E36" s="9"/>
     </row>
-    <row r="37" spans="2:5">
-      <c r="B37" s="42"/>
+    <row r="37" spans="2:5" ht="15">
+      <c r="B37" s="51"/>
       <c r="C37" s="4"/>
       <c r="D37" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E37" s="13" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5">
-      <c r="B38" s="42"/>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" ht="15">
+      <c r="B38" s="51"/>
       <c r="C38" s="4"/>
       <c r="D38" s="23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E38" s="13" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5">
-      <c r="B39" s="42"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" ht="15">
+      <c r="B39" s="51"/>
       <c r="C39" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D39" s="19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E39" s="26"/>
     </row>
-    <row r="40" spans="2:5">
-      <c r="B40" s="42"/>
+    <row r="40" spans="2:5" ht="15">
+      <c r="B40" s="51"/>
       <c r="C40" s="4" t="s">
         <v>33</v>
       </c>
@@ -2303,197 +2511,197 @@
       <c r="E40" s="9"/>
     </row>
     <row r="41" spans="2:5" ht="30">
-      <c r="B41" s="42"/>
+      <c r="B41" s="51"/>
       <c r="C41" s="4" t="s">
         <v>57</v>
       </c>
       <c r="D41" s="24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5">
-      <c r="B42" s="42"/>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" ht="15">
+      <c r="B42" s="51"/>
       <c r="C42" s="4" t="s">
         <v>34</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E42" s="9"/>
     </row>
     <row r="43" spans="2:5" ht="30">
-      <c r="B43" s="42"/>
+      <c r="B43" s="51"/>
       <c r="C43" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D43" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E43" s="13" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5">
-      <c r="B44" s="42"/>
+        <v>172</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" ht="15">
+      <c r="B44" s="51"/>
       <c r="C44" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D44" s="19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E44" s="9"/>
     </row>
     <row r="45" spans="2:5" ht="30.75" thickBot="1">
-      <c r="B45" s="42"/>
+      <c r="B45" s="51"/>
       <c r="C45" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D45" s="19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E45" s="13" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="46" spans="2:5" ht="30.75" thickBot="1">
-      <c r="B46" s="43"/>
+      <c r="B46" s="52"/>
       <c r="C46" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D46" s="25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E46" s="17" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="47" spans="2:5">
-      <c r="B47" s="34" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" ht="15">
+      <c r="B47" s="43" t="s">
         <v>39</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D47" s="35" t="s">
-        <v>79</v>
-      </c>
-      <c r="E47" s="40" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="48" spans="2:5">
-      <c r="B48" s="34"/>
+      <c r="D47" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="E47" s="49" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" ht="15">
+      <c r="B48" s="43"/>
       <c r="C48" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D48" s="36"/>
-      <c r="E48" s="40"/>
+      <c r="D48" s="45"/>
+      <c r="E48" s="49"/>
     </row>
     <row r="49" spans="2:5" ht="30">
-      <c r="B49" s="34"/>
+      <c r="B49" s="43"/>
       <c r="C49" s="4" t="s">
         <v>42</v>
       </c>
       <c r="D49" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5" ht="30">
-      <c r="B50" s="34" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" ht="28.5">
+      <c r="B50" s="43" t="s">
         <v>43</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>47</v>
       </c>
       <c r="D50" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5">
-      <c r="B51" s="34"/>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" ht="15">
+      <c r="B51" s="43"/>
       <c r="C51" s="4" t="s">
         <v>44</v>
       </c>
       <c r="D51" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="E51" s="37" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5">
-      <c r="B52" s="34"/>
+        <v>77</v>
+      </c>
+      <c r="E51" s="46" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" ht="15">
+      <c r="B52" s="43"/>
       <c r="C52" s="4" t="s">
         <v>64</v>
       </c>
       <c r="D52" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="E52" s="38"/>
-    </row>
-    <row r="53" spans="2:5">
-      <c r="B53" s="34"/>
+        <v>77</v>
+      </c>
+      <c r="E52" s="47"/>
+    </row>
+    <row r="53" spans="2:5" ht="15">
+      <c r="B53" s="43"/>
       <c r="C53" s="4" t="s">
         <v>46</v>
       </c>
       <c r="D53" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="E53" s="39"/>
+        <v>77</v>
+      </c>
+      <c r="E53" s="48"/>
     </row>
     <row r="54" spans="2:5" ht="30">
-      <c r="B54" s="34"/>
+      <c r="B54" s="43"/>
       <c r="C54" s="4" t="s">
         <v>45</v>
       </c>
       <c r="D54" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E54" s="13" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="55" spans="2:5" ht="30">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" ht="28.5">
       <c r="B55" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="C55" s="55" t="s">
+        <v>80</v>
+      </c>
+      <c r="C55" s="37" t="s">
+        <v>97</v>
+      </c>
+      <c r="D55" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="D55" s="56" t="s">
-        <v>99</v>
-      </c>
       <c r="E55" s="9"/>
     </row>
     <row r="56" spans="2:5">
-      <c r="B56" s="53" t="s">
+      <c r="B56" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="C56" s="36"/>
+      <c r="D56" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="C56" s="53"/>
-      <c r="D56" s="53" t="s">
-        <v>97</v>
-      </c>
-      <c r="E56" s="53"/>
+      <c r="E56" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="E51:E53"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="B28:B46"/>
     <mergeCell ref="B4:B6"/>
     <mergeCell ref="B7:B27"/>
     <mergeCell ref="B47:B49"/>
     <mergeCell ref="B50:B54"/>
     <mergeCell ref="D47:D48"/>
-    <mergeCell ref="E51:E53"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="B28:B46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -2505,18 +2713,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:E52"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B37" zoomScaleNormal="100" zoomScaleSheetLayoutView="93" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView showGridLines="0" topLeftCell="B19" zoomScaleNormal="100" zoomScaleSheetLayoutView="93" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="61.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="48.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="59.5703125" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="2.125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="17.875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="61.625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="48.125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="59.625" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="9.125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="10.5" customHeight="1"/>
@@ -2543,7 +2751,7 @@
       <c r="E3" s="9"/>
     </row>
     <row r="4" spans="2:5">
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="39" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -2554,8 +2762,8 @@
       </c>
       <c r="E4" s="9"/>
     </row>
-    <row r="5" spans="2:5" ht="30">
-      <c r="B5" s="44"/>
+    <row r="5" spans="2:5">
+      <c r="B5" s="39"/>
       <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
@@ -2563,11 +2771,11 @@
         <v>52</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="2:5">
-      <c r="B6" s="44"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="4" t="s">
         <v>6</v>
       </c>
@@ -2576,8 +2784,8 @@
       </c>
       <c r="E6" s="9"/>
     </row>
-    <row r="7" spans="2:5">
-      <c r="B7" s="45" t="s">
+    <row r="7" spans="2:5" ht="14.25">
+      <c r="B7" s="40" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="5" t="s">
@@ -2588,8 +2796,8 @@
       </c>
       <c r="E7" s="9"/>
     </row>
-    <row r="8" spans="2:5" ht="180">
-      <c r="B8" s="46"/>
+    <row r="8" spans="2:5" ht="171">
+      <c r="B8" s="41"/>
       <c r="C8" s="4" t="s">
         <v>55</v>
       </c>
@@ -2597,11 +2805,11 @@
         <v>53</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" ht="30">
-      <c r="B9" s="46"/>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="28.5">
+      <c r="B9" s="41"/>
       <c r="C9" s="4" t="s">
         <v>8</v>
       </c>
@@ -2613,7 +2821,7 @@
       </c>
     </row>
     <row r="10" spans="2:5">
-      <c r="B10" s="46"/>
+      <c r="B10" s="41"/>
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
@@ -2623,7 +2831,7 @@
       <c r="E10" s="9"/>
     </row>
     <row r="11" spans="2:5" ht="30">
-      <c r="B11" s="46"/>
+      <c r="B11" s="41"/>
       <c r="C11" s="4" t="s">
         <v>62</v>
       </c>
@@ -2634,8 +2842,8 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="2:5">
-      <c r="B12" s="46"/>
+    <row r="12" spans="2:5" ht="14.25">
+      <c r="B12" s="41"/>
       <c r="C12" s="5" t="s">
         <v>10</v>
       </c>
@@ -2645,7 +2853,7 @@
       <c r="E12" s="9"/>
     </row>
     <row r="13" spans="2:5">
-      <c r="B13" s="46"/>
+      <c r="B13" s="41"/>
       <c r="C13" s="4" t="s">
         <v>11</v>
       </c>
@@ -2657,7 +2865,7 @@
       </c>
     </row>
     <row r="14" spans="2:5">
-      <c r="B14" s="46"/>
+      <c r="B14" s="41"/>
       <c r="C14" s="4" t="s">
         <v>12</v>
       </c>
@@ -2669,7 +2877,7 @@
       </c>
     </row>
     <row r="15" spans="2:5">
-      <c r="B15" s="46"/>
+      <c r="B15" s="41"/>
       <c r="C15" s="4" t="s">
         <v>13</v>
       </c>
@@ -2681,7 +2889,7 @@
       </c>
     </row>
     <row r="16" spans="2:5">
-      <c r="B16" s="46"/>
+      <c r="B16" s="41"/>
       <c r="C16" s="4" t="s">
         <v>14</v>
       </c>
@@ -2692,8 +2900,8 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="45">
-      <c r="B17" s="46"/>
+    <row r="17" spans="2:5" ht="28.5">
+      <c r="B17" s="41"/>
       <c r="C17" s="4" t="s">
         <v>15</v>
       </c>
@@ -2701,11 +2909,11 @@
         <v>48</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5">
-      <c r="B18" s="46"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="14.25">
+      <c r="B18" s="41"/>
       <c r="C18" s="5" t="s">
         <v>16</v>
       </c>
@@ -2715,39 +2923,39 @@
       <c r="E18" s="9"/>
     </row>
     <row r="19" spans="2:5">
-      <c r="B19" s="46"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E19" s="37" t="s">
+      <c r="E19" s="46" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="20" spans="2:5">
-      <c r="B20" s="46"/>
+      <c r="B20" s="41"/>
       <c r="C20" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E20" s="38"/>
+      <c r="E20" s="47"/>
     </row>
     <row r="21" spans="2:5">
-      <c r="B21" s="46"/>
+      <c r="B21" s="41"/>
       <c r="C21" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E21" s="39"/>
-    </row>
-    <row r="22" spans="2:5">
-      <c r="B22" s="46"/>
+      <c r="E21" s="48"/>
+    </row>
+    <row r="22" spans="2:5" ht="14.25">
+      <c r="B22" s="41"/>
       <c r="C22" s="5" t="s">
         <v>20</v>
       </c>
@@ -2757,7 +2965,7 @@
       <c r="E22" s="9"/>
     </row>
     <row r="23" spans="2:5">
-      <c r="B23" s="46"/>
+      <c r="B23" s="41"/>
       <c r="C23" s="4" t="s">
         <v>21</v>
       </c>
@@ -2769,7 +2977,7 @@
       </c>
     </row>
     <row r="24" spans="2:5">
-      <c r="B24" s="47"/>
+      <c r="B24" s="42"/>
       <c r="C24" s="4" t="s">
         <v>22</v>
       </c>
@@ -2781,7 +2989,7 @@
       </c>
     </row>
     <row r="25" spans="2:5">
-      <c r="B25" s="34" t="s">
+      <c r="B25" s="43" t="s">
         <v>23</v>
       </c>
       <c r="C25" s="4" t="s">
@@ -2795,7 +3003,7 @@
       </c>
     </row>
     <row r="26" spans="2:5">
-      <c r="B26" s="34"/>
+      <c r="B26" s="43"/>
       <c r="C26" s="4" t="s">
         <v>25</v>
       </c>
@@ -2807,7 +3015,7 @@
       </c>
     </row>
     <row r="27" spans="2:5">
-      <c r="B27" s="34"/>
+      <c r="B27" s="43"/>
       <c r="C27" s="4" t="s">
         <v>26</v>
       </c>
@@ -2819,7 +3027,7 @@
       </c>
     </row>
     <row r="28" spans="2:5">
-      <c r="B28" s="34"/>
+      <c r="B28" s="43"/>
       <c r="C28" s="4" t="s">
         <v>27</v>
       </c>
@@ -2831,7 +3039,7 @@
       </c>
     </row>
     <row r="29" spans="2:5">
-      <c r="B29" s="34"/>
+      <c r="B29" s="43"/>
       <c r="C29" s="4" t="s">
         <v>28</v>
       </c>
@@ -2843,7 +3051,7 @@
       </c>
     </row>
     <row r="30" spans="2:5">
-      <c r="B30" s="34"/>
+      <c r="B30" s="43"/>
       <c r="C30" s="4" t="s">
         <v>29</v>
       </c>
@@ -2855,7 +3063,7 @@
       </c>
     </row>
     <row r="31" spans="2:5">
-      <c r="B31" s="34"/>
+      <c r="B31" s="43"/>
       <c r="C31" s="4" t="s">
         <v>30</v>
       </c>
@@ -2867,7 +3075,7 @@
       </c>
     </row>
     <row r="32" spans="2:5">
-      <c r="B32" s="34"/>
+      <c r="B32" s="43"/>
       <c r="C32" s="4" t="s">
         <v>31</v>
       </c>
@@ -2879,7 +3087,7 @@
       </c>
     </row>
     <row r="33" spans="2:5">
-      <c r="B33" s="34"/>
+      <c r="B33" s="43"/>
       <c r="C33" s="4" t="s">
         <v>32</v>
       </c>
@@ -2891,7 +3099,7 @@
       </c>
     </row>
     <row r="34" spans="2:5">
-      <c r="B34" s="34"/>
+      <c r="B34" s="43"/>
       <c r="C34" s="4" t="s">
         <v>33</v>
       </c>
@@ -2902,8 +3110,8 @@
         <v>72</v>
       </c>
     </row>
-    <row r="35" spans="2:5" ht="30">
-      <c r="B35" s="34"/>
+    <row r="35" spans="2:5">
+      <c r="B35" s="43"/>
       <c r="C35" s="4" t="s">
         <v>57</v>
       </c>
@@ -2915,7 +3123,7 @@
       </c>
     </row>
     <row r="36" spans="2:5">
-      <c r="B36" s="34"/>
+      <c r="B36" s="43"/>
       <c r="C36" s="4" t="s">
         <v>34</v>
       </c>
@@ -2927,7 +3135,7 @@
       </c>
     </row>
     <row r="37" spans="2:5" ht="30">
-      <c r="B37" s="34"/>
+      <c r="B37" s="43"/>
       <c r="C37" s="4" t="s">
         <v>35</v>
       </c>
@@ -2939,7 +3147,7 @@
       </c>
     </row>
     <row r="38" spans="2:5">
-      <c r="B38" s="34"/>
+      <c r="B38" s="43"/>
       <c r="C38" s="4" t="s">
         <v>36</v>
       </c>
@@ -2949,7 +3157,7 @@
       <c r="E38" s="13"/>
     </row>
     <row r="39" spans="2:5" ht="30">
-      <c r="B39" s="34"/>
+      <c r="B39" s="43"/>
       <c r="C39" s="4" t="s">
         <v>37</v>
       </c>
@@ -2958,8 +3166,8 @@
       </c>
       <c r="E39" s="27"/>
     </row>
-    <row r="40" spans="2:5" ht="30">
-      <c r="B40" s="34"/>
+    <row r="40" spans="2:5">
+      <c r="B40" s="43"/>
       <c r="C40" s="4" t="s">
         <v>38</v>
       </c>
@@ -2969,37 +3177,37 @@
       <c r="E40" s="27"/>
     </row>
     <row r="41" spans="2:5">
-      <c r="B41" s="34" t="s">
+      <c r="B41" s="43" t="s">
         <v>39</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>40</v>
       </c>
       <c r="D41" s="4"/>
-      <c r="E41" s="48" t="s">
-        <v>74</v>
+      <c r="E41" s="53" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="42" spans="2:5">
-      <c r="B42" s="34"/>
+      <c r="B42" s="43"/>
       <c r="C42" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D42" s="4"/>
-      <c r="E42" s="49"/>
+      <c r="E42" s="54"/>
     </row>
     <row r="43" spans="2:5">
-      <c r="B43" s="34"/>
+      <c r="B43" s="43"/>
       <c r="C43" s="4" t="s">
         <v>42</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E43" s="50"/>
+      <c r="E43" s="55"/>
     </row>
     <row r="44" spans="2:5">
-      <c r="B44" s="34" t="s">
+      <c r="B44" s="43" t="s">
         <v>43</v>
       </c>
       <c r="C44" s="4" t="s">
@@ -3013,7 +3221,7 @@
       </c>
     </row>
     <row r="45" spans="2:5">
-      <c r="B45" s="34"/>
+      <c r="B45" s="43"/>
       <c r="C45" s="4" t="s">
         <v>44</v>
       </c>
@@ -3024,8 +3232,8 @@
         <v>72</v>
       </c>
     </row>
-    <row r="46" spans="2:5" ht="30">
-      <c r="B46" s="34"/>
+    <row r="46" spans="2:5" ht="28.5">
+      <c r="B46" s="43"/>
       <c r="C46" s="4" t="s">
         <v>64</v>
       </c>
@@ -3036,8 +3244,8 @@
         <v>73</v>
       </c>
     </row>
-    <row r="47" spans="2:5" ht="30">
-      <c r="B47" s="34"/>
+    <row r="47" spans="2:5" ht="28.5">
+      <c r="B47" s="43"/>
       <c r="C47" s="4" t="s">
         <v>46</v>
       </c>
@@ -3049,7 +3257,7 @@
       </c>
     </row>
     <row r="48" spans="2:5">
-      <c r="B48" s="34"/>
+      <c r="B48" s="43"/>
       <c r="C48" s="4" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
modified:   "Hs ph\303\241t tri\341\273\203n s\341\272\243n ph\341\272\251m 5G Wifi/1. Router 4G Wifi/4G Wifi Huawei CPE vs No Huawei - technical compare (version 1).xlsb.xlsx" 	modified:   Part 1.docx 	"Hs ph\303\241t tri\341\273\203n s\341\272\243n ph\341\272\251m 5G Wifi/1. Router 4G Wifi/2. CPE 5G mobi spec.docx" "Hs ph\303\241t tri\341\273\203n s\341\272\243n ph\341\272\251m 5G Wifi/1. Router 4G Wifi/Device comparation and 5G CPE suggestion.xlsx" 	"Hs ph\303\241t tri\341\273\203n s\341\272\243n ph\341\272\251m 5G Wifi/CPE 5g/"
</commit_message>
<xml_diff>
--- a/Hs phát triển sản phẩm 5G Wifi/1. Router 4G Wifi/4G Wifi Huawei CPE vs No Huawei - technical compare (version 1).xlsb.xlsx
+++ b/Hs phát triển sản phẩm 5G Wifi/1. Router 4G Wifi/4G Wifi Huawei CPE vs No Huawei - technical compare (version 1).xlsb.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dzung\Desktop\mbf\thu_viec_mbf\Hs phát triển sản phẩm 5G Wifi\1. Router 4G Wifi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\My\Desktop\Dung\thử việc mbf\Hs phát triển sản phẩm 5G Wifi\1. Router 4G Wifi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{037B33EF-1AE9-4DA6-8A6E-C9D465B18999}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4956984A-2A5B-456B-99F1-1DA41D41B3F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="5G cpe " sheetId="4" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="208">
   <si>
     <t>Product model</t>
   </si>
@@ -415,7 +415,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -424,7 +424,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -434,7 +434,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -446,7 +446,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -456,7 +456,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -663,9 +663,6 @@
 -4G: B3,B7</t>
   </si>
   <si>
-    <t>N77, N78, N79, N41 là 3 băng tần được sử dụng để thử nghiệm 5G ở Việt Nam, hiện tại Mobifone đang thử nghiệm tại băng tần N41</t>
-  </si>
-  <si>
     <t>Button</t>
   </si>
   <si>
@@ -683,9 +680,6 @@
 - Speeds: 2.4GHz - 300Mbps, 5GHz - 867Mbps</t>
   </si>
   <si>
-    <t>antenna với 7 dbi cho độ phủ sóng cao</t>
-  </si>
-  <si>
     <t>Indicator</t>
   </si>
   <si>
@@ -702,53 +696,83 @@
 4 LAN indicator (Led or LCD)</t>
   </si>
   <si>
+    <t>Built-in antenna phù hợp hơn cho các Home Wifi vì độ phủ sóng đều hơn. Trong khi external antenna cho độ bao phủ mở rộng xa nhất từ phía nguồn phát.</t>
+  </si>
+  <si>
+    <t>SMS</t>
+  </si>
+  <si>
+    <t>IPv4/ipv6</t>
+  </si>
+  <si>
+    <t>CS/ VoLTE/ VoIP</t>
+  </si>
+  <si>
+    <t>1 power button
+1 reset button
+1 WPS button</t>
+  </si>
+  <si>
+    <t>1 led for 5G 
+1 led for 4G
+1 led for Wifi</t>
+  </si>
+  <si>
+    <t>IPv4 and IPv6/IPv4 dual stack</t>
+  </si>
+  <si>
+    <t>SMS service</t>
+  </si>
+  <si>
+    <t>firewall</t>
+  </si>
+  <si>
+    <t>PIN protection</t>
+  </si>
+  <si>
+    <t>MAC address filtering</t>
+  </si>
+  <si>
+    <t>VPN tunnel/VPN penetration</t>
+  </si>
+  <si>
+    <t>WebUI</t>
+  </si>
+  <si>
+    <t>VPN</t>
+  </si>
+  <si>
+    <t>App</t>
+  </si>
+  <si>
+    <t>Screen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 power button
+1 RECOVERY button
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4K video streaming, low latency for gaming </t>
+  </si>
+  <si>
+    <t>Intergrated display and speakers</t>
+  </si>
+  <si>
+    <t>IPv6 and IPv6/IPv4 dual stack</t>
+  </si>
+  <si>
+    <t>Firmware update</t>
+  </si>
+  <si>
+    <t>WPA, WPA2</t>
+  </si>
+  <si>
     <t>- 1 WAN GE port,
 - 4 LAN ports
 - 1 x SIM card slot(for Nano-SIM card)
-- 1 power adapter port</t>
-  </si>
-  <si>
-    <t>Built-in antenna phù hợp hơn cho các Home Wifi vì độ phủ sóng đều hơn. Trong khi external antenna cho độ bao phủ mở rộng xa nhất từ phía nguồn phát.</t>
-  </si>
-  <si>
-    <t>SMS</t>
-  </si>
-  <si>
-    <t>IPv4/ipv6</t>
-  </si>
-  <si>
-    <t>CS/ VoLTE/ VoIP</t>
-  </si>
-  <si>
-    <t>1 power button
-1 reset button
-1 WPS button</t>
-  </si>
-  <si>
-    <t>1 led for 5G 
-1 led for 4G
-1 led for Wifi</t>
-  </si>
-  <si>
-    <t>IPv4 and IPv6/IPv4 dual stack</t>
-  </si>
-  <si>
-    <t>SMS service</t>
-  </si>
-  <si>
-    <t>firewall</t>
-  </si>
-  <si>
-    <t>PIN protection</t>
-  </si>
-  <si>
-    <t>MAC address filtering</t>
-  </si>
-  <si>
-    <t>VPN tunnel/VPN penetration</t>
-  </si>
-  <si>
-    <t>WebUI</t>
+- 1 power adapter port
+- 1 external antenna</t>
   </si>
 </sst>
 </file>
@@ -759,7 +783,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -767,7 +791,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -806,7 +830,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -814,13 +838,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -856,24 +880,19 @@
       <family val="1"/>
     </font>
     <font>
-      <b/>
       <sz val="13"/>
-      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <name val="Arial"/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1016,7 +1035,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1120,14 +1139,59 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -1149,27 +1213,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1180,49 +1223,42 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1650,20 +1686,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFD3B9FB-EB72-43D1-8F21-9D6CE3B2B12D}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.75" customWidth="1"/>
-    <col min="4" max="4" width="50.25" customWidth="1"/>
-    <col min="5" max="5" width="47.125" style="10" customWidth="1"/>
-    <col min="6" max="6" width="33.25" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.7109375" customWidth="1"/>
+    <col min="4" max="4" width="50.28515625" customWidth="1"/>
+    <col min="5" max="5" width="47.140625" style="10" customWidth="1"/>
+    <col min="6" max="6" width="33.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="49.5">
@@ -1683,7 +1719,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16.5">
+    <row r="2" spans="1:6" ht="33">
       <c r="A2" s="30">
         <v>1</v>
       </c>
@@ -1696,11 +1732,11 @@
       <c r="D2" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="E2" s="56" t="s">
+      <c r="E2" s="38" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="181.5">
+    <row r="3" spans="1:6" ht="198">
       <c r="A3" s="30">
         <v>2</v>
       </c>
@@ -1713,12 +1749,10 @@
       <c r="D3" s="32" t="s">
         <v>133</v>
       </c>
-      <c r="E3" s="57" t="s">
+      <c r="E3" s="39" t="s">
         <v>176</v>
       </c>
-      <c r="F3" s="35" t="s">
-        <v>177</v>
-      </c>
+      <c r="F3" s="78"/>
     </row>
     <row r="4" spans="1:6" ht="16.5">
       <c r="A4" s="30">
@@ -1733,7 +1767,7 @@
       <c r="D4" s="31" t="s">
         <v>135</v>
       </c>
-      <c r="E4" s="56" t="s">
+      <c r="E4" s="38" t="s">
         <v>135</v>
       </c>
     </row>
@@ -1750,11 +1784,11 @@
       <c r="D5" s="32" t="s">
         <v>138</v>
       </c>
-      <c r="E5" s="57" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="33">
+      <c r="E5" s="39" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="49.5">
       <c r="A6" s="30">
         <v>5</v>
       </c>
@@ -1767,14 +1801,12 @@
       <c r="D6" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="E6" s="56" t="s">
+      <c r="E6" s="38" t="s">
         <v>140</v>
       </c>
-      <c r="F6" s="34" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="49.5">
+      <c r="F6" s="34"/>
+    </row>
+    <row r="7" spans="1:6" ht="66">
       <c r="A7" s="30">
         <v>6</v>
       </c>
@@ -1782,13 +1814,13 @@
         <v>141</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D7" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="E7" s="57" t="s">
-        <v>181</v>
+      <c r="E7" s="39" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="99">
@@ -1804,8 +1836,8 @@
       <c r="D8" s="32" t="s">
         <v>145</v>
       </c>
-      <c r="E8" s="57" t="s">
-        <v>187</v>
+      <c r="E8" s="39" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="33">
@@ -1821,7 +1853,7 @@
       <c r="D9" s="31" t="s">
         <v>147</v>
       </c>
-      <c r="E9" s="57" t="s">
+      <c r="E9" s="39" t="s">
         <v>148</v>
       </c>
     </row>
@@ -1838,7 +1870,7 @@
       <c r="D10" s="33">
         <v>20</v>
       </c>
-      <c r="E10" s="58">
+      <c r="E10" s="40">
         <v>50</v>
       </c>
     </row>
@@ -1855,7 +1887,7 @@
       <c r="D11" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="E11" s="57" t="s">
+      <c r="E11" s="39" t="s">
         <v>151</v>
       </c>
     </row>
@@ -1872,7 +1904,7 @@
       <c r="D12" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="E12" s="57" t="s">
+      <c r="E12" s="39" t="s">
         <v>154</v>
       </c>
     </row>
@@ -1889,7 +1921,7 @@
       <c r="D13" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="E13" s="56" t="s">
+      <c r="E13" s="38" t="s">
         <v>157</v>
       </c>
     </row>
@@ -1906,7 +1938,7 @@
       <c r="D14" s="31" t="s">
         <v>160</v>
       </c>
-      <c r="E14" s="56" t="s">
+      <c r="E14" s="38" t="s">
         <v>161</v>
       </c>
     </row>
@@ -1923,7 +1955,7 @@
       <c r="D15" s="31" t="s">
         <v>163</v>
       </c>
-      <c r="E15" s="56" t="s">
+      <c r="E15" s="38" t="s">
         <v>164</v>
       </c>
     </row>
@@ -1940,157 +1972,264 @@
       <c r="D16" s="31" t="s">
         <v>167</v>
       </c>
-      <c r="E16" s="56"/>
+      <c r="E16" s="38"/>
     </row>
     <row r="17" spans="1:5" ht="49.5">
-      <c r="A17" s="59">
+      <c r="A17" s="41">
         <v>15</v>
       </c>
-      <c r="B17" s="60" t="s">
-        <v>178</v>
-      </c>
-      <c r="C17" s="62" t="s">
+      <c r="B17" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="C17" s="70" t="s">
+        <v>189</v>
+      </c>
+      <c r="D17" s="70" t="s">
+        <v>201</v>
+      </c>
+      <c r="E17" s="64" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="49.5">
+      <c r="A18" s="41">
+        <v>16</v>
+      </c>
+      <c r="B18" s="42" t="s">
+        <v>181</v>
+      </c>
+      <c r="C18" s="70" t="s">
+        <v>190</v>
+      </c>
+      <c r="D18" s="37" t="s">
+        <v>200</v>
+      </c>
+      <c r="E18" s="64" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="16.5">
+      <c r="A19" s="44">
+        <v>17</v>
+      </c>
+      <c r="B19" s="66" t="s">
+        <v>182</v>
+      </c>
+      <c r="C19" s="71" t="s">
         <v>192</v>
       </c>
-      <c r="D17" s="36"/>
-      <c r="E17" s="61" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="49.5">
-      <c r="A18" s="59">
-        <v>16</v>
-      </c>
-      <c r="B18" s="60" t="s">
-        <v>183</v>
-      </c>
-      <c r="C18" s="62" t="s">
+      <c r="D19" s="70" t="s">
+        <v>186</v>
+      </c>
+      <c r="E19" s="64" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="16.5">
+      <c r="A20" s="45"/>
+      <c r="B20" s="67"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="64" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="16.5">
+      <c r="A21" s="45"/>
+      <c r="B21" s="67"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="64" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="16.5">
+      <c r="A22" s="45"/>
+      <c r="B22" s="67"/>
+      <c r="C22" s="69" t="s">
+        <v>119</v>
+      </c>
+      <c r="D22" s="69" t="s">
+        <v>119</v>
+      </c>
+      <c r="E22" s="65" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="16.5">
+      <c r="A23" s="45"/>
+      <c r="B23" s="67"/>
+      <c r="C23" s="71" t="s">
+        <v>191</v>
+      </c>
+      <c r="D23" s="71" t="s">
+        <v>204</v>
+      </c>
+      <c r="E23" s="64" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="16.5">
+      <c r="A24" s="45"/>
+      <c r="B24" s="67"/>
+      <c r="C24" s="69" t="s">
+        <v>88</v>
+      </c>
+      <c r="D24" s="69" t="s">
+        <v>88</v>
+      </c>
+      <c r="E24" s="65" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="16.5">
+      <c r="A25" s="45"/>
+      <c r="B25" s="67"/>
+      <c r="C25" s="70" t="s">
+        <v>206</v>
+      </c>
+      <c r="D25" s="70" t="s">
+        <v>206</v>
+      </c>
+      <c r="E25" s="64" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="16.5">
+      <c r="A26" s="45"/>
+      <c r="B26" s="67"/>
+      <c r="C26" s="70" t="s">
+        <v>188</v>
+      </c>
+      <c r="D26" s="37"/>
+      <c r="E26" s="64" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A27" s="45"/>
+      <c r="B27" s="67"/>
+      <c r="C27" s="72" t="s">
         <v>193</v>
       </c>
-      <c r="D18" s="36"/>
-      <c r="E18" s="61" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="16.5">
-      <c r="A19" s="67">
-        <v>17</v>
-      </c>
-      <c r="B19" s="64" t="s">
-        <v>184</v>
-      </c>
-      <c r="C19" s="70" t="s">
+      <c r="D27" s="72" t="s">
+        <v>193</v>
+      </c>
+      <c r="E27" s="74" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A28" s="45"/>
+      <c r="B28" s="67"/>
+      <c r="C28" s="72" t="s">
+        <v>194</v>
+      </c>
+      <c r="D28" s="72" t="s">
+        <v>194</v>
+      </c>
+      <c r="E28" s="74" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A29" s="45"/>
+      <c r="B29" s="67"/>
+      <c r="C29" s="72" t="s">
         <v>195</v>
       </c>
-      <c r="D19" s="36"/>
-      <c r="E19" s="61" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="16.5">
-      <c r="A20" s="68"/>
-      <c r="B20" s="65"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="61" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="16.5">
-      <c r="A21" s="68"/>
-      <c r="B21" s="65"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="61" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="16.5">
-      <c r="A22" s="68"/>
-      <c r="B22" s="65"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="63" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="16.5">
-      <c r="A23" s="68"/>
-      <c r="B23" s="65"/>
-      <c r="C23" s="71" t="s">
-        <v>194</v>
-      </c>
-      <c r="D23" s="36"/>
-      <c r="E23" s="61" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="16.5">
-      <c r="A24" s="68"/>
-      <c r="B24" s="65"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="63" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="16.5">
-      <c r="A25" s="68"/>
-      <c r="B25" s="65"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="61" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="16.5">
-      <c r="A26" s="69"/>
-      <c r="B26" s="66"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="61" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="15">
-      <c r="C27" s="70" t="s">
+      <c r="D29" s="72" t="s">
+        <v>195</v>
+      </c>
+      <c r="E29" s="74" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A30" s="45"/>
+      <c r="B30" s="67"/>
+      <c r="C30" s="72" t="s">
         <v>196</v>
       </c>
-      <c r="E27" s="70" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="15">
-      <c r="C28" s="70" t="s">
+      <c r="D30" s="72" t="s">
+        <v>198</v>
+      </c>
+      <c r="E30" s="75" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A31" s="45"/>
+      <c r="B31" s="67"/>
+      <c r="C31" s="72" t="s">
         <v>197</v>
       </c>
-      <c r="E28" s="70" t="s">
+      <c r="D31" s="72" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="15">
-      <c r="C29" s="70" t="s">
-        <v>198</v>
-      </c>
-      <c r="E29" s="70" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="15">
-      <c r="C30" s="70" t="s">
+      <c r="E31" s="74" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="16.5">
+      <c r="A32" s="45"/>
+      <c r="B32" s="67"/>
+      <c r="C32" s="73" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" ht="15">
-      <c r="C31" s="70" t="s">
-        <v>200</v>
-      </c>
+      <c r="D32" s="37" t="s">
+        <v>199</v>
+      </c>
+      <c r="E32" s="64" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="16.5">
+      <c r="A33" s="45"/>
+      <c r="B33" s="67"/>
+      <c r="C33" s="70" t="s">
+        <v>205</v>
+      </c>
+      <c r="D33" s="70" t="s">
+        <v>205</v>
+      </c>
+      <c r="E33" s="64" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="16.5">
+      <c r="A34" s="45"/>
+      <c r="B34" s="67"/>
+      <c r="C34" s="35"/>
+      <c r="D34" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="E34" s="43"/>
+    </row>
+    <row r="35" spans="1:5" ht="16.5">
+      <c r="A35" s="46"/>
+      <c r="B35" s="68"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="73" t="s">
+        <v>203</v>
+      </c>
+      <c r="E35" s="43"/>
+    </row>
+    <row r="37" spans="1:5" ht="16.5">
+      <c r="D37" s="76"/>
+    </row>
+    <row r="39" spans="1:5" ht="16.5">
+      <c r="D39" s="77"/>
+    </row>
+    <row r="40" spans="1:5" ht="16.5">
+      <c r="D40" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B19:B26"/>
-    <mergeCell ref="A19:A26"/>
+    <mergeCell ref="B19:B35"/>
+    <mergeCell ref="A19:A35"/>
   </mergeCells>
+  <phoneticPr fontId="17" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D1" r:id="rId1" display="https://www.htc.com/vn/5g/htc-5g-hub/)" xr:uid="{EC2AE463-2BA2-4A7E-AF7A-05AD3688B96E}"/>
   </hyperlinks>
@@ -2103,17 +2242,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B86DDA3-AC0A-4D94-B436-44C073F25763}">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51:E53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="18.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.75" customWidth="1"/>
-    <col min="4" max="4" width="51.875" customWidth="1"/>
-    <col min="5" max="5" width="53.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.7109375" customWidth="1"/>
+    <col min="4" max="4" width="51.85546875" customWidth="1"/>
+    <col min="5" max="5" width="53.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2142,8 +2281,8 @@
       <c r="C3" s="7"/>
       <c r="D3" s="18"/>
     </row>
-    <row r="4" spans="1:5" ht="15">
-      <c r="B4" s="39" t="s">
+    <row r="4" spans="1:5">
+      <c r="B4" s="54" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -2154,8 +2293,8 @@
       </c>
       <c r="E4" s="9"/>
     </row>
-    <row r="5" spans="1:5" ht="15">
-      <c r="B5" s="39"/>
+    <row r="5" spans="1:5" ht="30">
+      <c r="B5" s="54"/>
       <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
@@ -2166,8 +2305,8 @@
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15">
-      <c r="B6" s="39"/>
+    <row r="6" spans="1:5">
+      <c r="B6" s="54"/>
       <c r="C6" s="4" t="s">
         <v>6</v>
       </c>
@@ -2177,7 +2316,7 @@
       <c r="E6" s="9"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="55" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="14" t="s">
@@ -2188,8 +2327,8 @@
       </c>
       <c r="E7" s="9"/>
     </row>
-    <row r="8" spans="1:5" ht="15">
-      <c r="B8" s="41"/>
+    <row r="8" spans="1:5">
+      <c r="B8" s="56"/>
       <c r="C8" s="8" t="s">
         <v>77</v>
       </c>
@@ -2198,8 +2337,8 @@
       </c>
       <c r="E8" s="9"/>
     </row>
-    <row r="9" spans="1:5" ht="28.5">
-      <c r="B9" s="41"/>
+    <row r="9" spans="1:5" ht="30">
+      <c r="B9" s="56"/>
       <c r="C9" s="4" t="s">
         <v>55</v>
       </c>
@@ -2210,8 +2349,8 @@
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15">
-      <c r="B10" s="41"/>
+    <row r="10" spans="1:5">
+      <c r="B10" s="56"/>
       <c r="C10" s="4" t="s">
         <v>8</v>
       </c>
@@ -2221,7 +2360,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="30">
-      <c r="B11" s="41"/>
+      <c r="B11" s="56"/>
       <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
@@ -2233,7 +2372,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="30">
-      <c r="B12" s="41"/>
+      <c r="B12" s="56"/>
       <c r="C12" s="4" t="s">
         <v>62</v>
       </c>
@@ -2243,7 +2382,7 @@
       <c r="E12" s="9"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="B13" s="41"/>
+      <c r="B13" s="56"/>
       <c r="C13" s="14" t="s">
         <v>10</v>
       </c>
@@ -2252,8 +2391,8 @@
       </c>
       <c r="E13" s="9"/>
     </row>
-    <row r="14" spans="1:5" ht="15">
-      <c r="B14" s="41"/>
+    <row r="14" spans="1:5">
+      <c r="B14" s="56"/>
       <c r="C14" s="4" t="s">
         <v>11</v>
       </c>
@@ -2262,8 +2401,8 @@
       </c>
       <c r="E14" s="9"/>
     </row>
-    <row r="15" spans="1:5" ht="15">
-      <c r="B15" s="41"/>
+    <row r="15" spans="1:5">
+      <c r="B15" s="56"/>
       <c r="C15" s="4" t="s">
         <v>12</v>
       </c>
@@ -2272,8 +2411,8 @@
       </c>
       <c r="E15" s="9"/>
     </row>
-    <row r="16" spans="1:5" ht="15">
-      <c r="B16" s="41"/>
+    <row r="16" spans="1:5">
+      <c r="B16" s="56"/>
       <c r="C16" s="4" t="s">
         <v>13</v>
       </c>
@@ -2282,8 +2421,8 @@
       </c>
       <c r="E16" s="9"/>
     </row>
-    <row r="17" spans="2:5" ht="15">
-      <c r="B17" s="41"/>
+    <row r="17" spans="2:5">
+      <c r="B17" s="56"/>
       <c r="C17" s="4" t="s">
         <v>14</v>
       </c>
@@ -2292,8 +2431,8 @@
       </c>
       <c r="E17" s="9"/>
     </row>
-    <row r="18" spans="2:5" ht="15">
-      <c r="B18" s="41"/>
+    <row r="18" spans="2:5">
+      <c r="B18" s="56"/>
       <c r="C18" s="16" t="s">
         <v>77</v>
       </c>
@@ -2302,8 +2441,8 @@
       </c>
       <c r="E18" s="9"/>
     </row>
-    <row r="19" spans="2:5" ht="15">
-      <c r="B19" s="41"/>
+    <row r="19" spans="2:5">
+      <c r="B19" s="56"/>
       <c r="C19" s="16" t="s">
         <v>77</v>
       </c>
@@ -2312,8 +2451,8 @@
       </c>
       <c r="E19" s="9"/>
     </row>
-    <row r="20" spans="2:5" ht="15">
-      <c r="B20" s="41"/>
+    <row r="20" spans="2:5">
+      <c r="B20" s="56"/>
       <c r="C20" s="4" t="s">
         <v>15</v>
       </c>
@@ -2325,15 +2464,15 @@
       </c>
     </row>
     <row r="21" spans="2:5">
-      <c r="B21" s="41"/>
+      <c r="B21" s="56"/>
       <c r="C21" s="14" t="s">
         <v>16</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="9"/>
     </row>
-    <row r="22" spans="2:5" ht="15">
-      <c r="B22" s="41"/>
+    <row r="22" spans="2:5">
+      <c r="B22" s="56"/>
       <c r="C22" s="4" t="s">
         <v>17</v>
       </c>
@@ -2342,8 +2481,8 @@
       </c>
       <c r="E22" s="9"/>
     </row>
-    <row r="23" spans="2:5" ht="15">
-      <c r="B23" s="41"/>
+    <row r="23" spans="2:5">
+      <c r="B23" s="56"/>
       <c r="C23" s="4" t="s">
         <v>18</v>
       </c>
@@ -2352,8 +2491,8 @@
       </c>
       <c r="E23" s="9"/>
     </row>
-    <row r="24" spans="2:5" ht="15">
-      <c r="B24" s="41"/>
+    <row r="24" spans="2:5">
+      <c r="B24" s="56"/>
       <c r="C24" s="4" t="s">
         <v>19</v>
       </c>
@@ -2365,7 +2504,7 @@
       </c>
     </row>
     <row r="25" spans="2:5">
-      <c r="B25" s="41"/>
+      <c r="B25" s="56"/>
       <c r="C25" s="14" t="s">
         <v>20</v>
       </c>
@@ -2374,24 +2513,24 @@
       </c>
       <c r="E25" s="9"/>
     </row>
-    <row r="26" spans="2:5" ht="15">
-      <c r="B26" s="41"/>
+    <row r="26" spans="2:5">
+      <c r="B26" s="56"/>
       <c r="C26" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="19"/>
       <c r="E26" s="9"/>
     </row>
-    <row r="27" spans="2:5" ht="15">
-      <c r="B27" s="42"/>
+    <row r="27" spans="2:5">
+      <c r="B27" s="57"/>
       <c r="C27" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D27" s="19"/>
       <c r="E27" s="9"/>
     </row>
-    <row r="28" spans="2:5" ht="15">
-      <c r="B28" s="50" t="s">
+    <row r="28" spans="2:5">
+      <c r="B28" s="51" t="s">
         <v>23</v>
       </c>
       <c r="C28" s="16" t="s">
@@ -2402,8 +2541,8 @@
       </c>
       <c r="E28" s="9"/>
     </row>
-    <row r="29" spans="2:5" ht="15">
-      <c r="B29" s="51"/>
+    <row r="29" spans="2:5">
+      <c r="B29" s="52"/>
       <c r="C29" s="4" t="s">
         <v>24</v>
       </c>
@@ -2412,56 +2551,56 @@
       </c>
       <c r="E29" s="9"/>
     </row>
-    <row r="30" spans="2:5" ht="15">
-      <c r="B30" s="51"/>
+    <row r="30" spans="2:5">
+      <c r="B30" s="52"/>
       <c r="C30" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D30" s="19"/>
       <c r="E30" s="9"/>
     </row>
-    <row r="31" spans="2:5" ht="15">
-      <c r="B31" s="51"/>
+    <row r="31" spans="2:5">
+      <c r="B31" s="52"/>
       <c r="C31" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D31" s="19"/>
       <c r="E31" s="9"/>
     </row>
-    <row r="32" spans="2:5" ht="15">
-      <c r="B32" s="51"/>
+    <row r="32" spans="2:5">
+      <c r="B32" s="52"/>
       <c r="C32" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D32" s="19"/>
       <c r="E32" s="9"/>
     </row>
-    <row r="33" spans="2:5" ht="15">
-      <c r="B33" s="51"/>
+    <row r="33" spans="2:5">
+      <c r="B33" s="52"/>
       <c r="C33" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D33" s="19"/>
       <c r="E33" s="9"/>
     </row>
-    <row r="34" spans="2:5" ht="15">
-      <c r="B34" s="51"/>
+    <row r="34" spans="2:5">
+      <c r="B34" s="52"/>
       <c r="C34" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D34" s="19"/>
       <c r="E34" s="9"/>
     </row>
-    <row r="35" spans="2:5" ht="15">
-      <c r="B35" s="51"/>
+    <row r="35" spans="2:5">
+      <c r="B35" s="52"/>
       <c r="C35" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D35" s="19"/>
       <c r="E35" s="9"/>
     </row>
-    <row r="36" spans="2:5" ht="15">
-      <c r="B36" s="51"/>
+    <row r="36" spans="2:5">
+      <c r="B36" s="52"/>
       <c r="C36" s="4" t="s">
         <v>31</v>
       </c>
@@ -2470,8 +2609,8 @@
       </c>
       <c r="E36" s="9"/>
     </row>
-    <row r="37" spans="2:5" ht="15">
-      <c r="B37" s="51"/>
+    <row r="37" spans="2:5">
+      <c r="B37" s="52"/>
       <c r="C37" s="4"/>
       <c r="D37" s="23" t="s">
         <v>110</v>
@@ -2480,8 +2619,8 @@
         <v>113</v>
       </c>
     </row>
-    <row r="38" spans="2:5" ht="15">
-      <c r="B38" s="51"/>
+    <row r="38" spans="2:5">
+      <c r="B38" s="52"/>
       <c r="C38" s="4"/>
       <c r="D38" s="23" t="s">
         <v>111</v>
@@ -2490,8 +2629,8 @@
         <v>120</v>
       </c>
     </row>
-    <row r="39" spans="2:5" ht="15">
-      <c r="B39" s="51"/>
+    <row r="39" spans="2:5">
+      <c r="B39" s="52"/>
       <c r="C39" s="4" t="s">
         <v>32</v>
       </c>
@@ -2500,8 +2639,8 @@
       </c>
       <c r="E39" s="26"/>
     </row>
-    <row r="40" spans="2:5" ht="15">
-      <c r="B40" s="51"/>
+    <row r="40" spans="2:5">
+      <c r="B40" s="52"/>
       <c r="C40" s="4" t="s">
         <v>33</v>
       </c>
@@ -2511,7 +2650,7 @@
       <c r="E40" s="9"/>
     </row>
     <row r="41" spans="2:5" ht="30">
-      <c r="B41" s="51"/>
+      <c r="B41" s="52"/>
       <c r="C41" s="4" t="s">
         <v>57</v>
       </c>
@@ -2522,8 +2661,8 @@
         <v>92</v>
       </c>
     </row>
-    <row r="42" spans="2:5" ht="15">
-      <c r="B42" s="51"/>
+    <row r="42" spans="2:5">
+      <c r="B42" s="52"/>
       <c r="C42" s="4" t="s">
         <v>34</v>
       </c>
@@ -2533,7 +2672,7 @@
       <c r="E42" s="9"/>
     </row>
     <row r="43" spans="2:5" ht="30">
-      <c r="B43" s="51"/>
+      <c r="B43" s="52"/>
       <c r="C43" s="4" t="s">
         <v>35</v>
       </c>
@@ -2544,8 +2683,8 @@
         <v>172</v>
       </c>
     </row>
-    <row r="44" spans="2:5" ht="15">
-      <c r="B44" s="51"/>
+    <row r="44" spans="2:5">
+      <c r="B44" s="52"/>
       <c r="C44" s="4" t="s">
         <v>36</v>
       </c>
@@ -2555,7 +2694,7 @@
       <c r="E44" s="9"/>
     </row>
     <row r="45" spans="2:5" ht="30.75" thickBot="1">
-      <c r="B45" s="51"/>
+      <c r="B45" s="52"/>
       <c r="C45" s="4" t="s">
         <v>37</v>
       </c>
@@ -2567,7 +2706,7 @@
       </c>
     </row>
     <row r="46" spans="2:5" ht="30.75" thickBot="1">
-      <c r="B46" s="52"/>
+      <c r="B46" s="53"/>
       <c r="C46" s="4" t="s">
         <v>38</v>
       </c>
@@ -2578,30 +2717,30 @@
         <v>170</v>
       </c>
     </row>
-    <row r="47" spans="2:5" ht="15">
-      <c r="B47" s="43" t="s">
+    <row r="47" spans="2:5">
+      <c r="B47" s="58" t="s">
         <v>39</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D47" s="44" t="s">
+      <c r="D47" s="59" t="s">
         <v>78</v>
       </c>
-      <c r="E47" s="49" t="s">
+      <c r="E47" s="50" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="48" spans="2:5" ht="15">
-      <c r="B48" s="43"/>
+    <row r="48" spans="2:5">
+      <c r="B48" s="58"/>
       <c r="C48" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D48" s="45"/>
-      <c r="E48" s="49"/>
+      <c r="D48" s="60"/>
+      <c r="E48" s="50"/>
     </row>
     <row r="49" spans="2:5" ht="30">
-      <c r="B49" s="43"/>
+      <c r="B49" s="58"/>
       <c r="C49" s="4" t="s">
         <v>42</v>
       </c>
@@ -2612,8 +2751,8 @@
         <v>169</v>
       </c>
     </row>
-    <row r="50" spans="2:5" ht="28.5">
-      <c r="B50" s="43" t="s">
+    <row r="50" spans="2:5" ht="30">
+      <c r="B50" s="58" t="s">
         <v>43</v>
       </c>
       <c r="C50" s="4" t="s">
@@ -2626,40 +2765,40 @@
         <v>114</v>
       </c>
     </row>
-    <row r="51" spans="2:5" ht="15">
-      <c r="B51" s="43"/>
+    <row r="51" spans="2:5">
+      <c r="B51" s="58"/>
       <c r="C51" s="4" t="s">
         <v>44</v>
       </c>
       <c r="D51" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="E51" s="46" t="s">
+      <c r="E51" s="47" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="52" spans="2:5" ht="15">
-      <c r="B52" s="43"/>
+    <row r="52" spans="2:5">
+      <c r="B52" s="58"/>
       <c r="C52" s="4" t="s">
         <v>64</v>
       </c>
       <c r="D52" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="E52" s="47"/>
-    </row>
-    <row r="53" spans="2:5" ht="15">
-      <c r="B53" s="43"/>
+      <c r="E52" s="48"/>
+    </row>
+    <row r="53" spans="2:5">
+      <c r="B53" s="58"/>
       <c r="C53" s="4" t="s">
         <v>46</v>
       </c>
       <c r="D53" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="E53" s="48"/>
+      <c r="E53" s="49"/>
     </row>
     <row r="54" spans="2:5" ht="30">
-      <c r="B54" s="43"/>
+      <c r="B54" s="58"/>
       <c r="C54" s="4" t="s">
         <v>45</v>
       </c>
@@ -2670,27 +2809,27 @@
         <v>116</v>
       </c>
     </row>
-    <row r="55" spans="2:5" ht="28.5">
+    <row r="55" spans="2:5" ht="30">
       <c r="B55" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="C55" s="37" t="s">
+      <c r="C55" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="D55" s="38" t="s">
+      <c r="D55" s="37" t="s">
         <v>98</v>
       </c>
       <c r="E55" s="9"/>
     </row>
     <row r="56" spans="2:5">
-      <c r="B56" s="36" t="s">
+      <c r="B56" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="C56" s="36"/>
-      <c r="D56" s="36" t="s">
+      <c r="C56" s="35"/>
+      <c r="D56" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="E56" s="36"/>
+      <c r="E56" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2713,18 +2852,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:E52"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B19" zoomScaleNormal="100" zoomScaleSheetLayoutView="93" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView showGridLines="0" topLeftCell="B40" zoomScaleNormal="100" zoomScaleSheetLayoutView="93" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="17.875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="61.625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="48.125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="59.625" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="9.125" style="2"/>
+    <col min="1" max="1" width="2.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="61.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="48.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="59.5703125" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="10.5" customHeight="1"/>
@@ -2751,7 +2890,7 @@
       <c r="E3" s="9"/>
     </row>
     <row r="4" spans="2:5">
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="54" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -2762,8 +2901,8 @@
       </c>
       <c r="E4" s="9"/>
     </row>
-    <row r="5" spans="2:5">
-      <c r="B5" s="39"/>
+    <row r="5" spans="2:5" ht="30">
+      <c r="B5" s="54"/>
       <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
@@ -2775,7 +2914,7 @@
       </c>
     </row>
     <row r="6" spans="2:5">
-      <c r="B6" s="39"/>
+      <c r="B6" s="54"/>
       <c r="C6" s="4" t="s">
         <v>6</v>
       </c>
@@ -2784,8 +2923,8 @@
       </c>
       <c r="E6" s="9"/>
     </row>
-    <row r="7" spans="2:5" ht="14.25">
-      <c r="B7" s="40" t="s">
+    <row r="7" spans="2:5">
+      <c r="B7" s="55" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="5" t="s">
@@ -2796,8 +2935,8 @@
       </c>
       <c r="E7" s="9"/>
     </row>
-    <row r="8" spans="2:5" ht="171">
-      <c r="B8" s="41"/>
+    <row r="8" spans="2:5" ht="180">
+      <c r="B8" s="56"/>
       <c r="C8" s="4" t="s">
         <v>55</v>
       </c>
@@ -2808,8 +2947,8 @@
         <v>117</v>
       </c>
     </row>
-    <row r="9" spans="2:5" ht="28.5">
-      <c r="B9" s="41"/>
+    <row r="9" spans="2:5" ht="30">
+      <c r="B9" s="56"/>
       <c r="C9" s="4" t="s">
         <v>8</v>
       </c>
@@ -2821,7 +2960,7 @@
       </c>
     </row>
     <row r="10" spans="2:5">
-      <c r="B10" s="41"/>
+      <c r="B10" s="56"/>
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
@@ -2831,7 +2970,7 @@
       <c r="E10" s="9"/>
     </row>
     <row r="11" spans="2:5" ht="30">
-      <c r="B11" s="41"/>
+      <c r="B11" s="56"/>
       <c r="C11" s="4" t="s">
         <v>62</v>
       </c>
@@ -2842,8 +2981,8 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="2:5" ht="14.25">
-      <c r="B12" s="41"/>
+    <row r="12" spans="2:5">
+      <c r="B12" s="56"/>
       <c r="C12" s="5" t="s">
         <v>10</v>
       </c>
@@ -2853,7 +2992,7 @@
       <c r="E12" s="9"/>
     </row>
     <row r="13" spans="2:5">
-      <c r="B13" s="41"/>
+      <c r="B13" s="56"/>
       <c r="C13" s="4" t="s">
         <v>11</v>
       </c>
@@ -2865,7 +3004,7 @@
       </c>
     </row>
     <row r="14" spans="2:5">
-      <c r="B14" s="41"/>
+      <c r="B14" s="56"/>
       <c r="C14" s="4" t="s">
         <v>12</v>
       </c>
@@ -2877,7 +3016,7 @@
       </c>
     </row>
     <row r="15" spans="2:5">
-      <c r="B15" s="41"/>
+      <c r="B15" s="56"/>
       <c r="C15" s="4" t="s">
         <v>13</v>
       </c>
@@ -2889,7 +3028,7 @@
       </c>
     </row>
     <row r="16" spans="2:5">
-      <c r="B16" s="41"/>
+      <c r="B16" s="56"/>
       <c r="C16" s="4" t="s">
         <v>14</v>
       </c>
@@ -2900,8 +3039,8 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="28.5">
-      <c r="B17" s="41"/>
+    <row r="17" spans="2:5" ht="45">
+      <c r="B17" s="56"/>
       <c r="C17" s="4" t="s">
         <v>15</v>
       </c>
@@ -2912,8 +3051,8 @@
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="14.25">
-      <c r="B18" s="41"/>
+    <row r="18" spans="2:5">
+      <c r="B18" s="56"/>
       <c r="C18" s="5" t="s">
         <v>16</v>
       </c>
@@ -2923,39 +3062,39 @@
       <c r="E18" s="9"/>
     </row>
     <row r="19" spans="2:5">
-      <c r="B19" s="41"/>
+      <c r="B19" s="56"/>
       <c r="C19" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E19" s="46" t="s">
+      <c r="E19" s="47" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="20" spans="2:5">
-      <c r="B20" s="41"/>
+      <c r="B20" s="56"/>
       <c r="C20" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E20" s="47"/>
+      <c r="E20" s="48"/>
     </row>
     <row r="21" spans="2:5">
-      <c r="B21" s="41"/>
+      <c r="B21" s="56"/>
       <c r="C21" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E21" s="48"/>
-    </row>
-    <row r="22" spans="2:5" ht="14.25">
-      <c r="B22" s="41"/>
+      <c r="E21" s="49"/>
+    </row>
+    <row r="22" spans="2:5">
+      <c r="B22" s="56"/>
       <c r="C22" s="5" t="s">
         <v>20</v>
       </c>
@@ -2965,7 +3104,7 @@
       <c r="E22" s="9"/>
     </row>
     <row r="23" spans="2:5">
-      <c r="B23" s="41"/>
+      <c r="B23" s="56"/>
       <c r="C23" s="4" t="s">
         <v>21</v>
       </c>
@@ -2977,7 +3116,7 @@
       </c>
     </row>
     <row r="24" spans="2:5">
-      <c r="B24" s="42"/>
+      <c r="B24" s="57"/>
       <c r="C24" s="4" t="s">
         <v>22</v>
       </c>
@@ -2989,7 +3128,7 @@
       </c>
     </row>
     <row r="25" spans="2:5">
-      <c r="B25" s="43" t="s">
+      <c r="B25" s="58" t="s">
         <v>23</v>
       </c>
       <c r="C25" s="4" t="s">
@@ -3003,7 +3142,7 @@
       </c>
     </row>
     <row r="26" spans="2:5">
-      <c r="B26" s="43"/>
+      <c r="B26" s="58"/>
       <c r="C26" s="4" t="s">
         <v>25</v>
       </c>
@@ -3015,7 +3154,7 @@
       </c>
     </row>
     <row r="27" spans="2:5">
-      <c r="B27" s="43"/>
+      <c r="B27" s="58"/>
       <c r="C27" s="4" t="s">
         <v>26</v>
       </c>
@@ -3027,7 +3166,7 @@
       </c>
     </row>
     <row r="28" spans="2:5">
-      <c r="B28" s="43"/>
+      <c r="B28" s="58"/>
       <c r="C28" s="4" t="s">
         <v>27</v>
       </c>
@@ -3039,7 +3178,7 @@
       </c>
     </row>
     <row r="29" spans="2:5">
-      <c r="B29" s="43"/>
+      <c r="B29" s="58"/>
       <c r="C29" s="4" t="s">
         <v>28</v>
       </c>
@@ -3051,7 +3190,7 @@
       </c>
     </row>
     <row r="30" spans="2:5">
-      <c r="B30" s="43"/>
+      <c r="B30" s="58"/>
       <c r="C30" s="4" t="s">
         <v>29</v>
       </c>
@@ -3063,7 +3202,7 @@
       </c>
     </row>
     <row r="31" spans="2:5">
-      <c r="B31" s="43"/>
+      <c r="B31" s="58"/>
       <c r="C31" s="4" t="s">
         <v>30</v>
       </c>
@@ -3075,7 +3214,7 @@
       </c>
     </row>
     <row r="32" spans="2:5">
-      <c r="B32" s="43"/>
+      <c r="B32" s="58"/>
       <c r="C32" s="4" t="s">
         <v>31</v>
       </c>
@@ -3087,7 +3226,7 @@
       </c>
     </row>
     <row r="33" spans="2:5">
-      <c r="B33" s="43"/>
+      <c r="B33" s="58"/>
       <c r="C33" s="4" t="s">
         <v>32</v>
       </c>
@@ -3099,7 +3238,7 @@
       </c>
     </row>
     <row r="34" spans="2:5">
-      <c r="B34" s="43"/>
+      <c r="B34" s="58"/>
       <c r="C34" s="4" t="s">
         <v>33</v>
       </c>
@@ -3110,8 +3249,8 @@
         <v>72</v>
       </c>
     </row>
-    <row r="35" spans="2:5">
-      <c r="B35" s="43"/>
+    <row r="35" spans="2:5" ht="30">
+      <c r="B35" s="58"/>
       <c r="C35" s="4" t="s">
         <v>57</v>
       </c>
@@ -3123,7 +3262,7 @@
       </c>
     </row>
     <row r="36" spans="2:5">
-      <c r="B36" s="43"/>
+      <c r="B36" s="58"/>
       <c r="C36" s="4" t="s">
         <v>34</v>
       </c>
@@ -3135,7 +3274,7 @@
       </c>
     </row>
     <row r="37" spans="2:5" ht="30">
-      <c r="B37" s="43"/>
+      <c r="B37" s="58"/>
       <c r="C37" s="4" t="s">
         <v>35</v>
       </c>
@@ -3147,7 +3286,7 @@
       </c>
     </row>
     <row r="38" spans="2:5">
-      <c r="B38" s="43"/>
+      <c r="B38" s="58"/>
       <c r="C38" s="4" t="s">
         <v>36</v>
       </c>
@@ -3157,7 +3296,7 @@
       <c r="E38" s="13"/>
     </row>
     <row r="39" spans="2:5" ht="30">
-      <c r="B39" s="43"/>
+      <c r="B39" s="58"/>
       <c r="C39" s="4" t="s">
         <v>37</v>
       </c>
@@ -3166,8 +3305,8 @@
       </c>
       <c r="E39" s="27"/>
     </row>
-    <row r="40" spans="2:5">
-      <c r="B40" s="43"/>
+    <row r="40" spans="2:5" ht="30">
+      <c r="B40" s="58"/>
       <c r="C40" s="4" t="s">
         <v>38</v>
       </c>
@@ -3177,37 +3316,37 @@
       <c r="E40" s="27"/>
     </row>
     <row r="41" spans="2:5">
-      <c r="B41" s="43" t="s">
+      <c r="B41" s="58" t="s">
         <v>39</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>40</v>
       </c>
       <c r="D41" s="4"/>
-      <c r="E41" s="53" t="s">
-        <v>188</v>
+      <c r="E41" s="61" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="42" spans="2:5">
-      <c r="B42" s="43"/>
+      <c r="B42" s="58"/>
       <c r="C42" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D42" s="4"/>
-      <c r="E42" s="54"/>
+      <c r="E42" s="62"/>
     </row>
     <row r="43" spans="2:5">
-      <c r="B43" s="43"/>
+      <c r="B43" s="58"/>
       <c r="C43" s="4" t="s">
         <v>42</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E43" s="55"/>
+      <c r="E43" s="63"/>
     </row>
     <row r="44" spans="2:5">
-      <c r="B44" s="43" t="s">
+      <c r="B44" s="58" t="s">
         <v>43</v>
       </c>
       <c r="C44" s="4" t="s">
@@ -3221,7 +3360,7 @@
       </c>
     </row>
     <row r="45" spans="2:5">
-      <c r="B45" s="43"/>
+      <c r="B45" s="58"/>
       <c r="C45" s="4" t="s">
         <v>44</v>
       </c>
@@ -3232,8 +3371,8 @@
         <v>72</v>
       </c>
     </row>
-    <row r="46" spans="2:5" ht="28.5">
-      <c r="B46" s="43"/>
+    <row r="46" spans="2:5" ht="30">
+      <c r="B46" s="58"/>
       <c r="C46" s="4" t="s">
         <v>64</v>
       </c>
@@ -3244,8 +3383,8 @@
         <v>73</v>
       </c>
     </row>
-    <row r="47" spans="2:5" ht="28.5">
-      <c r="B47" s="43"/>
+    <row r="47" spans="2:5" ht="30">
+      <c r="B47" s="58"/>
       <c r="C47" s="4" t="s">
         <v>46</v>
       </c>
@@ -3257,7 +3396,7 @@
       </c>
     </row>
     <row r="48" spans="2:5">
-      <c r="B48" s="43"/>
+      <c r="B48" s="58"/>
       <c r="C48" s="4" t="s">
         <v>45</v>
       </c>

</xml_diff>